<commit_message>
Eliminación de archivos innecesarios
</commit_message>
<xml_diff>
--- a/iave-web-api/middlewares/Asignación OrigenDestino inmediato por caseta.xlsx
+++ b/iave-web-api/middlewares/Asignación OrigenDestino inmediato por caseta.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="1173">
   <si>
     <t>Id_caseta</t>
   </si>
@@ -3523,6 +3523,21 @@
   </si>
   <si>
     <t>303667 </t>
+  </si>
+  <si>
+    <t>35390 </t>
+  </si>
+  <si>
+    <t>64301 </t>
+  </si>
+  <si>
+    <t>216095 </t>
+  </si>
+  <si>
+    <t>287640 </t>
+  </si>
+  <si>
+    <t>198944 </t>
   </si>
 </sst>
 </file>
@@ -3954,8 +3969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A769" workbookViewId="0">
-      <selection activeCell="H776" sqref="A776:J781"/>
+    <sheetView tabSelected="1" topLeftCell="A1002" workbookViewId="0">
+      <selection activeCell="D1012" sqref="A1009:J1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14794,6 +14809,12 @@
       <c r="C335" t="b">
         <v>1</v>
       </c>
+      <c r="D335" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E335">
+        <v>261329</v>
+      </c>
       <c r="F335">
         <v>20.72888</v>
       </c>
@@ -14824,6 +14845,12 @@
       <c r="C336" t="b">
         <v>1</v>
       </c>
+      <c r="D336" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E336">
+        <v>261329</v>
+      </c>
       <c r="F336">
         <v>20.72888</v>
       </c>
@@ -14854,6 +14881,12 @@
       <c r="C337" t="b">
         <v>0</v>
       </c>
+      <c r="D337" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E337">
+        <v>261329</v>
+      </c>
       <c r="F337">
         <v>20.72888</v>
       </c>
@@ -14884,6 +14917,12 @@
       <c r="C338" t="b">
         <v>0</v>
       </c>
+      <c r="D338" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E338">
+        <v>261329</v>
+      </c>
       <c r="F338">
         <v>20.72888</v>
       </c>
@@ -14914,6 +14953,12 @@
       <c r="C339" t="b">
         <v>1</v>
       </c>
+      <c r="D339" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E339">
+        <v>261329</v>
+      </c>
       <c r="F339">
         <v>20.72888</v>
       </c>
@@ -25924,6 +25969,12 @@
       <c r="C782" t="b">
         <v>1</v>
       </c>
+      <c r="D782" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E782">
+        <v>163321</v>
+      </c>
       <c r="F782">
         <v>19.925989999999999</v>
       </c>
@@ -25948,6 +25999,12 @@
       <c r="C783" t="b">
         <v>1</v>
       </c>
+      <c r="D783" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E783">
+        <v>182234</v>
+      </c>
       <c r="F783">
         <v>19.926220000000001</v>
       </c>
@@ -25972,6 +26029,12 @@
       <c r="C784" t="b">
         <v>1</v>
       </c>
+      <c r="D784">
+        <v>35390</v>
+      </c>
+      <c r="E784">
+        <v>42554</v>
+      </c>
       <c r="F784">
         <v>19.92643</v>
       </c>
@@ -25996,6 +26059,12 @@
       <c r="C785" t="b">
         <v>0</v>
       </c>
+      <c r="D785">
+        <v>35390</v>
+      </c>
+      <c r="E785">
+        <v>42554</v>
+      </c>
       <c r="F785">
         <v>19.92643</v>
       </c>
@@ -26020,6 +26089,12 @@
       <c r="C786" t="b">
         <v>0</v>
       </c>
+      <c r="D786">
+        <v>35390</v>
+      </c>
+      <c r="E786">
+        <v>166654</v>
+      </c>
       <c r="F786">
         <v>19.926100000000002</v>
       </c>
@@ -26044,6 +26119,12 @@
       <c r="C787" t="b">
         <v>0</v>
       </c>
+      <c r="D787">
+        <v>35390</v>
+      </c>
+      <c r="E787">
+        <v>166654</v>
+      </c>
       <c r="F787">
         <v>19.926100000000002</v>
       </c>
@@ -26068,6 +26149,12 @@
       <c r="C788" t="b">
         <v>1</v>
       </c>
+      <c r="D788" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E788">
+        <v>275979</v>
+      </c>
       <c r="F788">
         <v>19.926300000000001</v>
       </c>
@@ -26092,6 +26179,12 @@
       <c r="C789" t="b">
         <v>1</v>
       </c>
+      <c r="D789" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E789">
+        <v>275979</v>
+      </c>
       <c r="F789">
         <v>19.926300000000001</v>
       </c>
@@ -26260,6 +26353,12 @@
       <c r="C796" t="b">
         <v>0</v>
       </c>
+      <c r="D796" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E796">
+        <v>158701</v>
+      </c>
       <c r="F796">
         <v>19.081710000000001</v>
       </c>
@@ -26284,6 +26383,12 @@
       <c r="C797" t="b">
         <v>1</v>
       </c>
+      <c r="D797" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E797">
+        <v>158701</v>
+      </c>
       <c r="F797">
         <v>19.081710000000001</v>
       </c>
@@ -26308,6 +26413,12 @@
       <c r="C798" t="b">
         <v>1</v>
       </c>
+      <c r="D798" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E798">
+        <v>211672</v>
+      </c>
       <c r="F798">
         <v>18.226500000000001</v>
       </c>
@@ -26332,6 +26443,12 @@
       <c r="C799" t="b">
         <v>0</v>
       </c>
+      <c r="D799" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E799">
+        <v>211672</v>
+      </c>
       <c r="F799">
         <v>18.226500000000001</v>
       </c>
@@ -26692,6 +26809,12 @@
       <c r="C814" t="b">
         <v>1</v>
       </c>
+      <c r="D814" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E814">
+        <v>199234</v>
+      </c>
       <c r="F814">
         <v>25.448090000000001</v>
       </c>
@@ -26716,6 +26839,12 @@
       <c r="C815" t="b">
         <v>0</v>
       </c>
+      <c r="D815" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E815">
+        <v>199234</v>
+      </c>
       <c r="F815">
         <v>25.448090000000001</v>
       </c>
@@ -26740,6 +26869,12 @@
       <c r="C816" t="b">
         <v>1</v>
       </c>
+      <c r="D816" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E816">
+        <v>199234</v>
+      </c>
       <c r="F816">
         <v>25.448090000000001</v>
       </c>
@@ -26764,6 +26899,12 @@
       <c r="C817" t="b">
         <v>1</v>
       </c>
+      <c r="D817" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E817">
+        <v>199234</v>
+      </c>
       <c r="F817">
         <v>25.448090000000001</v>
       </c>
@@ -31372,6 +31513,12 @@
       <c r="C1009" t="b">
         <v>0</v>
       </c>
+      <c r="D1009" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E1009">
+        <v>243775</v>
+      </c>
       <c r="F1009">
         <v>20.515550000000001</v>
       </c>
@@ -31396,6 +31543,12 @@
       <c r="C1010" t="b">
         <v>1</v>
       </c>
+      <c r="D1010" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E1010">
+        <v>243775</v>
+      </c>
       <c r="F1010">
         <v>20.515550000000001</v>
       </c>
@@ -31420,6 +31573,12 @@
       <c r="C1011" t="b">
         <v>1</v>
       </c>
+      <c r="D1011" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E1011">
+        <v>243775</v>
+      </c>
       <c r="F1011">
         <v>20.515550000000001</v>
       </c>
@@ -31443,6 +31602,12 @@
       </c>
       <c r="C1012" t="b">
         <v>1</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E1012">
+        <v>243775</v>
       </c>
       <c r="F1012">
         <v>20.515550000000001</v>

</xml_diff>

<commit_message>
Implementación: Actualización de la gestión y el enrutamiento de casetas
- Se refactorizaron las rutas en `rutas_casetas.routes.js` para incluir un nuevo endpoint para obtener y actualizar los detalles de las casetas.
- Se añadió una ruta para actualizar casetas en `App.js`.
- Se mejoró `Route-Creator.jsx` para gestionar la normalización de ubicaciones adicionales y la lógica de obtención de datos.
- Se modificó `CasetasTable.jsx` para integrar un modal para actualizar los detalles de las casetas, incluyendo una nueva gestión de estado para la visibilidad modal y el ID de caseta seleccionada.
- Se implementó `ModalUpdateCaseta` en `utils.jsx` para actualizar los costos de las casetas con una lógica de obtención de datos y validación de campos.
- Se eliminaron componentes no utilizados y se limpió el código en `nuevocomponente.jsx`.
</commit_message>
<xml_diff>
--- a/iave-web-api/middlewares/Asignación OrigenDestino inmediato por caseta.xlsx
+++ b/iave-web-api/middlewares/Asignación OrigenDestino inmediato por caseta.xlsx
@@ -3673,7 +3673,11 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J1133" totalsRowShown="0">
-  <autoFilter ref="A1:J1133"/>
+  <autoFilter ref="A1:J1133">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" name="Id_caseta"/>
     <tableColumn id="2" name="NombreRelacionado"/>
@@ -3969,8 +3973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1002" workbookViewId="0">
-      <selection activeCell="D1012" sqref="A1009:J1012"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,7 +4031,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4063,7 +4067,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4099,7 +4103,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4135,7 +4139,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4475,7 +4479,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -4511,7 +4515,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -4547,7 +4551,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -4583,7 +4587,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -4655,7 +4659,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -4691,7 +4695,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -4817,7 +4821,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
@@ -4853,7 +4857,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
@@ -4889,7 +4893,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -4925,7 +4929,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>16</v>
       </c>
@@ -4961,7 +4965,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>17</v>
       </c>
@@ -4997,7 +5001,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -5033,7 +5037,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>19</v>
       </c>
@@ -5069,7 +5073,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
@@ -5105,7 +5109,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -5143,7 +5147,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20</v>
       </c>
@@ -5181,7 +5185,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>25</v>
       </c>
@@ -5217,7 +5221,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>26</v>
       </c>
@@ -5253,7 +5257,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>26</v>
       </c>
@@ -5619,7 +5623,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>33</v>
       </c>
@@ -5655,7 +5659,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>33</v>
       </c>
@@ -5691,7 +5695,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>33</v>
       </c>
@@ -5727,7 +5731,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>35</v>
       </c>
@@ -5763,7 +5767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>35</v>
       </c>
@@ -6039,7 +6043,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>43</v>
       </c>
@@ -6075,7 +6079,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>43</v>
       </c>
@@ -6111,7 +6115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>43</v>
       </c>
@@ -6147,7 +6151,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>44</v>
       </c>
@@ -6183,7 +6187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>44</v>
       </c>
@@ -6219,7 +6223,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>44</v>
       </c>
@@ -6255,7 +6259,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>45</v>
       </c>
@@ -6291,7 +6295,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>45</v>
       </c>
@@ -6327,7 +6331,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6363,7 +6367,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>46</v>
       </c>
@@ -6399,7 +6403,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>46</v>
       </c>
@@ -6435,7 +6439,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>46</v>
       </c>
@@ -6501,7 +6505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>49</v>
       </c>
@@ -6537,7 +6541,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>49</v>
       </c>
@@ -6573,7 +6577,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>49</v>
       </c>
@@ -6609,7 +6613,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>50</v>
       </c>
@@ -6645,7 +6649,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>50</v>
       </c>
@@ -6681,7 +6685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>51</v>
       </c>
@@ -6717,7 +6721,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>51</v>
       </c>
@@ -6753,7 +6757,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>52</v>
       </c>
@@ -6789,7 +6793,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>52</v>
       </c>
@@ -6825,7 +6829,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>53</v>
       </c>
@@ -6861,7 +6865,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>53</v>
       </c>
@@ -6897,7 +6901,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>56</v>
       </c>
@@ -6933,7 +6937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>56</v>
       </c>
@@ -6969,7 +6973,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>57</v>
       </c>
@@ -7005,7 +7009,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>57</v>
       </c>
@@ -7041,7 +7045,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>58</v>
       </c>
@@ -7077,7 +7081,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>58</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>58</v>
       </c>
@@ -7149,7 +7153,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>59</v>
       </c>
@@ -7185,7 +7189,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>59</v>
       </c>
@@ -7221,7 +7225,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>59</v>
       </c>
@@ -7257,7 +7261,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>60</v>
       </c>
@@ -7293,7 +7297,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>60</v>
       </c>
@@ -7329,7 +7333,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>60</v>
       </c>
@@ -7365,7 +7369,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>60</v>
       </c>
@@ -7401,7 +7405,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>63</v>
       </c>
@@ -7437,7 +7441,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>63</v>
       </c>
@@ -7473,7 +7477,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>66</v>
       </c>
@@ -7509,7 +7513,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>66</v>
       </c>
@@ -7665,7 +7669,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>68</v>
       </c>
@@ -7701,7 +7705,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>68</v>
       </c>
@@ -7737,7 +7741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>68</v>
       </c>
@@ -7773,7 +7777,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>68</v>
       </c>
@@ -7809,7 +7813,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>69</v>
       </c>
@@ -7845,7 +7849,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>69</v>
       </c>
@@ -7881,7 +7885,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>69</v>
       </c>
@@ -7947,7 +7951,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>71</v>
       </c>
@@ -7983,7 +7987,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>71</v>
       </c>
@@ -8019,7 +8023,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>72</v>
       </c>
@@ -8055,7 +8059,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>72</v>
       </c>
@@ -8091,7 +8095,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>73</v>
       </c>
@@ -8127,7 +8131,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>73</v>
       </c>
@@ -8163,7 +8167,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>74</v>
       </c>
@@ -8199,7 +8203,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>75</v>
       </c>
@@ -8235,7 +8239,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>75</v>
       </c>
@@ -8271,7 +8275,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>76</v>
       </c>
@@ -8307,7 +8311,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>76</v>
       </c>
@@ -8343,7 +8347,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>77</v>
       </c>
@@ -8379,7 +8383,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>77</v>
       </c>
@@ -8415,7 +8419,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>77</v>
       </c>
@@ -8541,7 +8545,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>81</v>
       </c>
@@ -8577,7 +8581,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>81</v>
       </c>
@@ -8613,7 +8617,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>81</v>
       </c>
@@ -8709,7 +8713,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>83</v>
       </c>
@@ -8745,7 +8749,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>83</v>
       </c>
@@ -8781,7 +8785,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>83</v>
       </c>
@@ -8913,7 +8917,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>85</v>
       </c>
@@ -8949,7 +8953,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>85</v>
       </c>
@@ -8985,7 +8989,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>85</v>
       </c>
@@ -9021,7 +9025,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>88</v>
       </c>
@@ -9057,7 +9061,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>88</v>
       </c>
@@ -9093,7 +9097,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>90</v>
       </c>
@@ -9279,7 +9283,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>94</v>
       </c>
@@ -9315,7 +9319,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>94</v>
       </c>
@@ -9351,7 +9355,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>94</v>
       </c>
@@ -9387,7 +9391,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>95</v>
       </c>
@@ -9423,7 +9427,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>95</v>
       </c>
@@ -9459,7 +9463,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>95</v>
       </c>
@@ -9585,7 +9589,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>97</v>
       </c>
@@ -9621,7 +9625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>97</v>
       </c>
@@ -9657,7 +9661,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>98</v>
       </c>
@@ -9693,7 +9697,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>98</v>
       </c>
@@ -9789,7 +9793,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>102</v>
       </c>
@@ -9825,7 +9829,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>102</v>
       </c>
@@ -9861,7 +9865,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>104</v>
       </c>
@@ -9897,7 +9901,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>104</v>
       </c>
@@ -10083,7 +10087,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="7">
         <v>107</v>
       </c>
@@ -10121,7 +10125,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>107</v>
       </c>
@@ -10157,7 +10161,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>107</v>
       </c>
@@ -10223,7 +10227,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>109</v>
       </c>
@@ -10259,7 +10263,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>111</v>
       </c>
@@ -10387,7 +10391,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>114</v>
       </c>
@@ -10425,7 +10429,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>114</v>
       </c>
@@ -10463,7 +10467,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>118</v>
       </c>
@@ -10501,7 +10505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>118</v>
       </c>
@@ -14799,7 +14803,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>226</v>
       </c>
@@ -14835,7 +14839,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>226</v>
       </c>
@@ -14871,7 +14875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>226</v>
       </c>
@@ -14907,7 +14911,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>226</v>
       </c>
@@ -14943,7 +14947,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>226</v>
       </c>
@@ -25599,7 +25603,7 @@
       </c>
       <c r="J767" s="5"/>
     </row>
-    <row r="768" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="768" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A768">
         <v>696</v>
       </c>
@@ -25629,7 +25633,7 @@
       </c>
       <c r="J768" s="5"/>
     </row>
-    <row r="769" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A769">
         <v>697</v>
       </c>
@@ -25707,7 +25711,7 @@
       </c>
       <c r="J771" s="5"/>
     </row>
-    <row r="772" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772">
         <v>703</v>
       </c>
@@ -25737,7 +25741,7 @@
       </c>
       <c r="J772" s="5"/>
     </row>
-    <row r="773" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773">
         <v>703</v>
       </c>
@@ -25959,7 +25963,7 @@
       </c>
       <c r="J781" s="5"/>
     </row>
-    <row r="782" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A782">
         <v>714</v>
       </c>
@@ -25989,7 +25993,7 @@
       </c>
       <c r="J782" s="5"/>
     </row>
-    <row r="783" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A783">
         <v>715</v>
       </c>
@@ -26019,7 +26023,7 @@
       </c>
       <c r="J783" s="5"/>
     </row>
-    <row r="784" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A784">
         <v>716</v>
       </c>
@@ -26049,7 +26053,7 @@
       </c>
       <c r="J784" s="5"/>
     </row>
-    <row r="785" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A785">
         <v>716</v>
       </c>
@@ -26079,7 +26083,7 @@
       </c>
       <c r="J785" s="5"/>
     </row>
-    <row r="786" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A786">
         <v>717</v>
       </c>
@@ -26109,7 +26113,7 @@
       </c>
       <c r="J786" s="5"/>
     </row>
-    <row r="787" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787">
         <v>717</v>
       </c>
@@ -26139,7 +26143,7 @@
       </c>
       <c r="J787" s="5"/>
     </row>
-    <row r="788" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788">
         <v>719</v>
       </c>
@@ -26169,7 +26173,7 @@
       </c>
       <c r="J788" s="5"/>
     </row>
-    <row r="789" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A789">
         <v>719</v>
       </c>
@@ -26343,7 +26347,7 @@
       </c>
       <c r="J795" s="5"/>
     </row>
-    <row r="796" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796">
         <v>727</v>
       </c>
@@ -26373,7 +26377,7 @@
       </c>
       <c r="J796" s="5"/>
     </row>
-    <row r="797" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A797">
         <v>727</v>
       </c>
@@ -26403,7 +26407,7 @@
       </c>
       <c r="J797" s="5"/>
     </row>
-    <row r="798" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A798">
         <v>728</v>
       </c>
@@ -26433,7 +26437,7 @@
       </c>
       <c r="J798" s="5"/>
     </row>
-    <row r="799" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A799">
         <v>728</v>
       </c>
@@ -26799,7 +26803,7 @@
       </c>
       <c r="J813" s="5"/>
     </row>
-    <row r="814" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A814">
         <v>733</v>
       </c>
@@ -26829,7 +26833,7 @@
       </c>
       <c r="J814" s="5"/>
     </row>
-    <row r="815" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A815">
         <v>733</v>
       </c>
@@ -26859,7 +26863,7 @@
       </c>
       <c r="J815" s="5"/>
     </row>
-    <row r="816" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A816">
         <v>733</v>
       </c>
@@ -26889,7 +26893,7 @@
       </c>
       <c r="J816" s="5"/>
     </row>
-    <row r="817" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817">
         <v>733</v>
       </c>
@@ -31503,7 +31507,7 @@
       </c>
       <c r="J1008" s="5"/>
     </row>
-    <row r="1009" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1009" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1009">
         <v>858</v>
       </c>
@@ -31533,7 +31537,7 @@
       </c>
       <c r="J1009" s="5"/>
     </row>
-    <row r="1010" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1010" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1010">
         <v>858</v>
       </c>
@@ -31563,7 +31567,7 @@
       </c>
       <c r="J1010" s="5"/>
     </row>
-    <row r="1011" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1011" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1011">
         <v>858</v>
       </c>
@@ -31593,7 +31597,7 @@
       </c>
       <c r="J1011" s="5"/>
     </row>
-    <row r="1012" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1012" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1012">
         <v>858</v>
       </c>

</xml_diff>